<commit_message>
Fitted skewnorms to data
</commit_message>
<xml_diff>
--- a/data/Experimental_data_Ed_Josh.xlsx
+++ b/data/Experimental_data_Ed_Josh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuamiller/Documents/Python Files/HCMV_Dose_Infection/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBAC2F7-E52F-584E-9513-44ACF6F0299D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CC8300-9449-584F-B95F-4456C828ED80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="28560" windowHeight="15040" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="28560" windowHeight="15040" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021_10_05 TB_GFP_epithelial" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="196">
   <si>
     <t>Cells</t>
   </si>
@@ -571,54 +571,6 @@
     <t>d.nm</t>
   </si>
   <si>
-    <t>Mean_1</t>
-  </si>
-  <si>
-    <t>sd_1</t>
-  </si>
-  <si>
-    <t>Mean_4</t>
-  </si>
-  <si>
-    <t>SD_4</t>
-  </si>
-  <si>
-    <t>Mean_7</t>
-  </si>
-  <si>
-    <t>SD_7</t>
-  </si>
-  <si>
-    <t>Mean_10</t>
-  </si>
-  <si>
-    <t>SD_10</t>
-  </si>
-  <si>
-    <t>Mean_13</t>
-  </si>
-  <si>
-    <t>SD_13</t>
-  </si>
-  <si>
-    <t>Mean_16</t>
-  </si>
-  <si>
-    <t>SD_16</t>
-  </si>
-  <si>
-    <t>Mean_19</t>
-  </si>
-  <si>
-    <t>SD_19</t>
-  </si>
-  <si>
-    <t>Mean_23</t>
-  </si>
-  <si>
-    <t>SD_23</t>
-  </si>
-  <si>
     <t>mCherry+</t>
   </si>
   <si>
@@ -629,6 +581,54 @@
   </si>
   <si>
     <t>Sample #</t>
+  </si>
+  <si>
+    <t>Mean_15240000</t>
+  </si>
+  <si>
+    <t>sd_15240000</t>
+  </si>
+  <si>
+    <t>Mean_6131312</t>
+  </si>
+  <si>
+    <t>SD_6131312</t>
+  </si>
+  <si>
+    <t>Mean_2450310</t>
+  </si>
+  <si>
+    <t>SD_2450310</t>
+  </si>
+  <si>
+    <t>Mean_972623</t>
+  </si>
+  <si>
+    <t>SD_972623</t>
+  </si>
+  <si>
+    <t>Mean_383425</t>
+  </si>
+  <si>
+    <t>SD_383425</t>
+  </si>
+  <si>
+    <t>Mean_150101</t>
+  </si>
+  <si>
+    <t>SD_150101</t>
+  </si>
+  <si>
+    <t>Mean_58345</t>
+  </si>
+  <si>
+    <t>SD_58345</t>
+  </si>
+  <si>
+    <t>Mean_16367</t>
+  </si>
+  <si>
+    <t>SD_16367</t>
   </si>
 </sst>
 </file>
@@ -13379,7 +13379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC77BCC-D392-B64F-91BD-E2C798404F90}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -13398,10 +13398,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>148</v>
@@ -13419,7 +13419,7 @@
         <v>127</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>148</v>
@@ -13463,7 +13463,7 @@
         <v>250</v>
       </c>
       <c r="L2" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -15591,8 +15591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8369BE0-C5E0-014C-BBD9-3FC0E79B5E41}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17963,68 +17963,95 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1386F1BF-0E77-EA49-9DC1-2DEFFACA1B2C}">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:U73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="H56" workbookViewId="0">
+      <selection activeCell="U73" sqref="U73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="G1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="H1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="I1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="J1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="K1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="L1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="M1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="N1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="O1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="P1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="Q1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+      <c r="S1" t="s">
+        <v>126</v>
+      </c>
+      <c r="T1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.4</v>
       </c>
@@ -18076,8 +18103,17 @@
       <c r="Q2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T2" s="2">
+        <v>89.647058823529406</v>
+      </c>
+      <c r="U2" s="3">
+        <v>15240000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.4632</v>
       </c>
@@ -18129,8 +18165,17 @@
       <c r="Q3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S3">
+        <v>1.2</v>
+      </c>
+      <c r="T3" s="2">
+        <v>89.647058823529406</v>
+      </c>
+      <c r="U3" s="3">
+        <v>15240000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.53649999999999998</v>
       </c>
@@ -18182,8 +18227,17 @@
       <c r="Q4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S4">
+        <v>1.3</v>
+      </c>
+      <c r="T4" s="2">
+        <v>89.647058823529406</v>
+      </c>
+      <c r="U4" s="3">
+        <v>15240000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.62129999999999996</v>
       </c>
@@ -18235,8 +18289,17 @@
       <c r="Q5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S5">
+        <v>2.1</v>
+      </c>
+      <c r="T5" s="2">
+        <v>66.228545875848624</v>
+      </c>
+      <c r="U5" s="3">
+        <v>11258852.798894266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.71950000000000003</v>
       </c>
@@ -18288,8 +18351,17 @@
       <c r="Q6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T6" s="2">
+        <v>66.228545875848624</v>
+      </c>
+      <c r="U6" s="3">
+        <v>11258852.798894266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.83320000000000005</v>
       </c>
@@ -18341,8 +18413,17 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T7" s="2">
+        <v>66.228545875848624</v>
+      </c>
+      <c r="U7" s="3">
+        <v>11258852.798894266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.96489999999999998</v>
       </c>
@@ -18394,8 +18475,17 @@
       <c r="Q8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S8">
+        <v>3.1</v>
+      </c>
+      <c r="T8" s="2">
+        <v>48.891710459594613</v>
+      </c>
+      <c r="U8" s="3">
+        <v>8311590.7781310836</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1.117</v>
       </c>
@@ -18447,8 +18537,17 @@
       <c r="Q9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S9">
+        <v>3.2</v>
+      </c>
+      <c r="T9" s="2">
+        <v>48.891710459594613</v>
+      </c>
+      <c r="U9" s="3">
+        <v>8311590.7781310836</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1.294</v>
       </c>
@@ -18500,8 +18599,17 @@
       <c r="Q10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S10">
+        <v>3.3</v>
+      </c>
+      <c r="T10" s="2">
+        <v>48.891710459594613</v>
+      </c>
+      <c r="U10" s="3">
+        <v>8311590.7781310836</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1.4990000000000001</v>
       </c>
@@ -18553,8 +18661,17 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="T11" s="2">
+        <v>36.066542830360213</v>
+      </c>
+      <c r="U11" s="3">
+        <v>6131312.2811612403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1.736</v>
       </c>
@@ -18606,8 +18723,17 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S12">
+        <v>4.2</v>
+      </c>
+      <c r="T12" s="2">
+        <v>36.066542830360213</v>
+      </c>
+      <c r="U12" s="3">
+        <v>6131312.2811612366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2.0099999999999998</v>
       </c>
@@ -18659,8 +18785,17 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S13">
+        <v>4.3</v>
+      </c>
+      <c r="T13" s="2">
+        <v>36.066542830360213</v>
+      </c>
+      <c r="U13" s="3">
+        <v>6131312.2811612366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2.3279999999999998</v>
       </c>
@@ -18712,8 +18847,17 @@
       <c r="Q14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="T14" s="2">
+        <v>26.58590778872172</v>
+      </c>
+      <c r="U14" s="3">
+        <v>4519604.3240826922</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2.6960000000000002</v>
       </c>
@@ -18765,8 +18909,17 @@
       <c r="Q15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S15">
+        <v>5.2</v>
+      </c>
+      <c r="T15" s="2">
+        <v>26.58590778872172</v>
+      </c>
+      <c r="U15" s="3">
+        <v>4519604.3240826922</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3.1219999999999999</v>
       </c>
@@ -18818,8 +18971,17 @@
       <c r="Q16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S16">
+        <v>5.3</v>
+      </c>
+      <c r="T16" s="2">
+        <v>26.58590778872172</v>
+      </c>
+      <c r="U16" s="3">
+        <v>4519604.3240826922</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3.6150000000000002</v>
       </c>
@@ -18871,8 +19033,17 @@
       <c r="Q17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S17">
+        <v>6.1</v>
+      </c>
+      <c r="T17" s="2">
+        <v>19.582790615107214</v>
+      </c>
+      <c r="U17" s="3">
+        <v>3329074.4045682265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4.1870000000000003</v>
       </c>
@@ -18924,8 +19095,17 @@
       <c r="Q18">
         <v>5.7735026918962581E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S18">
+        <v>6.2</v>
+      </c>
+      <c r="T18" s="2">
+        <v>19.582790615107214</v>
+      </c>
+      <c r="U18" s="3">
+        <v>3329074.4045682265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4.8490000000000002</v>
       </c>
@@ -18977,8 +19157,17 @@
       <c r="Q19">
         <v>0.15275252316519444</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S19">
+        <v>6.3</v>
+      </c>
+      <c r="T19" s="2">
+        <v>19.582790615107214</v>
+      </c>
+      <c r="U19" s="3">
+        <v>3329074.4045682265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5.6150000000000002</v>
       </c>
@@ -19030,8 +19219,17 @@
       <c r="Q20">
         <v>0.3055050463303885</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S20">
+        <v>7.1</v>
+      </c>
+      <c r="T20" s="2">
+        <v>14.413590299108243</v>
+      </c>
+      <c r="U20" s="3">
+        <v>2450310.3508484014</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6.5030000000000001</v>
       </c>
@@ -19083,8 +19281,17 @@
       <c r="Q21">
         <v>0.52915026221291916</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S21">
+        <v>7.2</v>
+      </c>
+      <c r="T21" s="2">
+        <v>14.413590299108243</v>
+      </c>
+      <c r="U21" s="3">
+        <v>2450310.3508484014</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7.5309999999999997</v>
       </c>
@@ -19136,8 +19343,17 @@
       <c r="Q22">
         <v>0.63508529610858766</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S22">
+        <v>7.3</v>
+      </c>
+      <c r="T22" s="2">
+        <v>14.413590299108243</v>
+      </c>
+      <c r="U22" s="3">
+        <v>2450310.3508484014</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8.7210000000000001</v>
       </c>
@@ -19189,8 +19405,17 @@
       <c r="Q23">
         <v>0.69999999999999629</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S23">
+        <v>8.1</v>
+      </c>
+      <c r="T23" s="2">
+        <v>10.600898113619849</v>
+      </c>
+      <c r="U23" s="3">
+        <v>1802152.6793153742</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>10.1</v>
       </c>
@@ -19242,8 +19467,17 @@
       <c r="Q24">
         <v>0.56862407030773654</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S24">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="T24" s="2">
+        <v>10.600898113619849</v>
+      </c>
+      <c r="U24" s="3">
+        <v>1802152.6793153742</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>11.7</v>
       </c>
@@ -19295,8 +19529,17 @@
       <c r="Q25">
         <v>0.35118845842842472</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S25">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="T25" s="2">
+        <v>10.600898113619849</v>
+      </c>
+      <c r="U25" s="3">
+        <v>1802152.6793153742</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>13.54</v>
       </c>
@@ -19348,8 +19591,17 @@
       <c r="Q26">
         <v>0.11547005383792526</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S26">
+        <v>9.1</v>
+      </c>
+      <c r="T26" s="2">
+        <v>7.7908423724218805</v>
+      </c>
+      <c r="U26" s="3">
+        <v>1324443.2033117197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>15.69</v>
       </c>
@@ -19401,8 +19653,17 @@
       <c r="Q27">
         <v>0.28867513459481287</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S27">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="T27" s="2">
+        <v>7.7908423724218805</v>
+      </c>
+      <c r="U27" s="3">
+        <v>1324443.2033117197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>18.170000000000002</v>
       </c>
@@ -19454,8 +19715,17 @@
       <c r="Q28">
         <v>0.51316014394468834</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S28">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="T28" s="2">
+        <v>7.7908423724218805</v>
+      </c>
+      <c r="U28" s="3">
+        <v>1324443.2033117197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>21.04</v>
       </c>
@@ -19507,8 +19777,17 @@
       <c r="Q29">
         <v>0.60277137733417663</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S29">
+        <v>10.1</v>
+      </c>
+      <c r="T29" s="2">
+        <v>5.7213143212795963</v>
+      </c>
+      <c r="U29" s="3">
+        <v>972623.43461753137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>24.36</v>
       </c>
@@ -19560,8 +19839,17 @@
       <c r="Q30">
         <v>0.556776436283002</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S30">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="T30" s="2">
+        <v>5.7213143212795963</v>
+      </c>
+      <c r="U30" s="3">
+        <v>972623.43461753137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28.21</v>
       </c>
@@ -19613,8 +19901,17 @@
       <c r="Q31">
         <v>0.46188021535170054</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S31">
+        <v>10.3</v>
+      </c>
+      <c r="T31" s="2">
+        <v>5.7213143212795963</v>
+      </c>
+      <c r="U31" s="3">
+        <v>972623.43461753137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>32.67</v>
       </c>
@@ -19666,8 +19963,17 @@
       <c r="Q32">
         <v>0.45092497528228959</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S32">
+        <v>11.1</v>
+      </c>
+      <c r="T32" s="2">
+        <v>4.1983165653333376</v>
+      </c>
+      <c r="U32" s="3">
+        <v>713713.81610666739</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>37.840000000000003</v>
       </c>
@@ -19719,8 +20025,17 @@
       <c r="Q33">
         <v>0.46188021535170048</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S33">
+        <v>11.2</v>
+      </c>
+      <c r="T33" s="2">
+        <v>4.1983165653333376</v>
+      </c>
+      <c r="U33" s="3">
+        <v>713713.81610666739</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>43.82</v>
       </c>
@@ -19772,8 +20087,17 @@
       <c r="Q34">
         <v>0.50332229568471676</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S34">
+        <v>11.3</v>
+      </c>
+      <c r="T34" s="2">
+        <v>4.1983165653333376</v>
+      </c>
+      <c r="U34" s="3">
+        <v>713713.81610666739</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>50.75</v>
       </c>
@@ -19825,8 +20149,17 @@
       <c r="Q35">
         <v>0.60277137733416786</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S35">
+        <v>12.1</v>
+      </c>
+      <c r="T35" s="2">
+        <v>3.0783704385189399</v>
+      </c>
+      <c r="U35" s="3">
+        <v>523322.97454821976</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>58.77</v>
       </c>
@@ -19878,8 +20211,17 @@
       <c r="Q36">
         <v>0.56862407030773343</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S36">
+        <v>12.2</v>
+      </c>
+      <c r="T36" s="2">
+        <v>3.0783704385189399</v>
+      </c>
+      <c r="U36" s="3">
+        <v>523322.97454821976</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>68.06</v>
       </c>
@@ -19931,8 +20273,17 @@
       <c r="Q37">
         <v>0.49328828623162008</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S37">
+        <v>12.3</v>
+      </c>
+      <c r="T37" s="2">
+        <v>3.0783704385189399</v>
+      </c>
+      <c r="U37" s="3">
+        <v>523322.97454821976</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>78.819999999999993</v>
       </c>
@@ -19984,8 +20335,17 @@
       <c r="Q38">
         <v>0.32145502536643189</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S38">
+        <v>13.1</v>
+      </c>
+      <c r="T38" s="2">
+        <v>2.2554397272316984</v>
+      </c>
+      <c r="U38" s="3">
+        <v>383424.75362938875</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>91.28</v>
       </c>
@@ -20037,8 +20397,17 @@
       <c r="Q39">
         <v>0.1732050807568879</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S39">
+        <v>13.2</v>
+      </c>
+      <c r="T39" s="2">
+        <v>2.2554397272316984</v>
+      </c>
+      <c r="U39" s="3">
+        <v>383424.75362938875</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>105.7</v>
       </c>
@@ -20090,8 +20459,17 @@
       <c r="Q40">
         <v>0.23094010767585024</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S40">
+        <v>13.3</v>
+      </c>
+      <c r="T40" s="2">
+        <v>2.2554397272316984</v>
+      </c>
+      <c r="U40" s="3">
+        <v>383424.75362938875</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>122.4</v>
       </c>
@@ -20143,8 +20521,17 @@
       <c r="Q41">
         <v>0.39999999999999797</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S41">
+        <v>14.1</v>
+      </c>
+      <c r="T41" s="2">
+        <v>1.6512184537422709</v>
+      </c>
+      <c r="U41" s="3">
+        <v>280707.13713618607</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>141.80000000000001</v>
       </c>
@@ -20196,8 +20583,17 @@
       <c r="Q42">
         <v>0.55677643628300189</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S42">
+        <v>14.2</v>
+      </c>
+      <c r="T42" s="2">
+        <v>1.6512184537422709</v>
+      </c>
+      <c r="U42" s="3">
+        <v>280707.13713618607</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>164.2</v>
       </c>
@@ -20249,8 +20645,17 @@
       <c r="Q43">
         <v>0.6658328118479393</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S43">
+        <v>14.3</v>
+      </c>
+      <c r="T43" s="2">
+        <v>1.6512184537422709</v>
+      </c>
+      <c r="U43" s="3">
+        <v>280707.13713618607</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>190.1</v>
       </c>
@@ -20302,8 +20707,17 @@
       <c r="Q44">
         <v>0.77674534651540306</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S44">
+        <v>15.1</v>
+      </c>
+      <c r="T44" s="2">
+        <v>1.2079225904506672</v>
+      </c>
+      <c r="U44" s="3">
+        <v>205346.84037661343</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>220.2</v>
       </c>
@@ -20355,8 +20769,17 @@
       <c r="Q45">
         <v>0.79372539331937753</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S45">
+        <v>15.2</v>
+      </c>
+      <c r="T45" s="2">
+        <v>1.2079225904506672</v>
+      </c>
+      <c r="U45" s="3">
+        <v>205346.84037661343</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>255</v>
       </c>
@@ -20408,8 +20831,17 @@
       <c r="Q46">
         <v>0.75718777944003646</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S46">
+        <v>15.3</v>
+      </c>
+      <c r="T46" s="2">
+        <v>1.2079225904506672</v>
+      </c>
+      <c r="U46" s="3">
+        <v>205346.84037661343</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>295.3</v>
       </c>
@@ -20461,8 +20893,17 @@
       <c r="Q47">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S47">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="T47" s="2">
+        <v>0.88294412839347702</v>
+      </c>
+      <c r="U47" s="3">
+        <v>150100.50182689109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>342</v>
       </c>
@@ -20514,8 +20955,17 @@
       <c r="Q48">
         <v>0.58594652770823141</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S48">
+        <v>16.2</v>
+      </c>
+      <c r="T48" s="2">
+        <v>0.88294412839347702</v>
+      </c>
+      <c r="U48" s="3">
+        <v>150100.50182689109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>396.1</v>
       </c>
@@ -20567,8 +21017,17 @@
       <c r="Q49">
         <v>0.4163331998932267</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S49">
+        <v>16.3</v>
+      </c>
+      <c r="T49" s="2">
+        <v>0.88294412839347702</v>
+      </c>
+      <c r="U49" s="3">
+        <v>150100.50182689109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>458.7</v>
       </c>
@@ -20620,8 +21079,17 @@
       <c r="Q50">
         <v>0.30550504633038933</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S50">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="T50" s="2">
+        <v>0.64488929206485057</v>
+      </c>
+      <c r="U50" s="3">
+        <v>109631.17965102459</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>531.20000000000005</v>
       </c>
@@ -20673,8 +21141,17 @@
       <c r="Q51">
         <v>0.25166114784235838</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S51">
+        <v>17.2</v>
+      </c>
+      <c r="T51" s="2">
+        <v>0.64488929206485057</v>
+      </c>
+      <c r="U51" s="3">
+        <v>109631.17965102459</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>615.1</v>
       </c>
@@ -20726,8 +21203,17 @@
       <c r="Q52">
         <v>0.20816659994661355</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S52">
+        <v>17.3</v>
+      </c>
+      <c r="T52" s="2">
+        <v>0.64488929206485057</v>
+      </c>
+      <c r="U52" s="3">
+        <v>109631.17965102459</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>712.4</v>
       </c>
@@ -20779,8 +21265,17 @@
       <c r="Q53">
         <v>0.25166114784235832</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S53">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="T53" s="2">
+        <v>0.47064472280072367</v>
+      </c>
+      <c r="U53" s="3">
+        <v>80009.602876123026</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>825</v>
       </c>
@@ -20832,8 +21327,17 @@
       <c r="Q54">
         <v>0.26457513110645903</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S54">
+        <v>18.2</v>
+      </c>
+      <c r="T54" s="2">
+        <v>0.47064472280072367</v>
+      </c>
+      <c r="U54" s="3">
+        <v>80009.602876123026</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>955.4</v>
       </c>
@@ -20885,8 +21389,17 @@
       <c r="Q55">
         <v>0.32145502536643183</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S55">
+        <v>18.3</v>
+      </c>
+      <c r="T55" s="2">
+        <v>0.47064472280072367</v>
+      </c>
+      <c r="U55" s="3">
+        <v>80009.602876123026</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1106</v>
       </c>
@@ -20938,8 +21451,17 @@
       <c r="Q56">
         <v>0.34641016151377546</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S56">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="T56" s="2">
+        <v>0.34320653854665945</v>
+      </c>
+      <c r="U56" s="3">
+        <v>58345.111552932103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1281</v>
       </c>
@@ -20991,8 +21513,17 @@
       <c r="Q57">
         <v>0.34641016151377546</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S57">
+        <v>19.2</v>
+      </c>
+      <c r="T57" s="2">
+        <v>0.34320653854665945</v>
+      </c>
+      <c r="U57" s="3">
+        <v>58345.111552932103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1484</v>
       </c>
@@ -21044,8 +21575,17 @@
       <c r="Q58">
         <v>0.28867513459481292</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S58">
+        <v>19.3</v>
+      </c>
+      <c r="T58" s="2">
+        <v>0.34320653854665945</v>
+      </c>
+      <c r="U58" s="3">
+        <v>58345.111552932103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1718</v>
       </c>
@@ -21097,8 +21637,17 @@
       <c r="Q59">
         <v>0.26457513110645908</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S59">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="T59" s="2">
+        <v>0.25007511602646043</v>
+      </c>
+      <c r="U59" s="3">
+        <v>42512.76972449827</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1990</v>
       </c>
@@ -21150,8 +21699,17 @@
       <c r="Q60">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S60">
+        <v>20.2</v>
+      </c>
+      <c r="T60" s="2">
+        <v>0.25007511602646043</v>
+      </c>
+      <c r="U60" s="3">
+        <v>42512.76972449827</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2305</v>
       </c>
@@ -21203,8 +21761,17 @@
       <c r="Q61">
         <v>0.17320508075688773</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S61">
+        <v>20.3</v>
+      </c>
+      <c r="T61" s="2">
+        <v>0.25007511602646043</v>
+      </c>
+      <c r="U61" s="3">
+        <v>42512.76972449827</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2669</v>
       </c>
@@ -21256,8 +21823,17 @@
       <c r="Q62">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S62">
+        <v>21.1</v>
+      </c>
+      <c r="T62" s="2">
+        <v>0.18206907727969637</v>
+      </c>
+      <c r="U62" s="3">
+        <v>30951.743137548383</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>3091</v>
       </c>
@@ -21309,8 +21885,17 @@
       <c r="Q63">
         <v>0.25166114784235838</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S63">
+        <v>21.2</v>
+      </c>
+      <c r="T63" s="2">
+        <v>0.18206907727969637</v>
+      </c>
+      <c r="U63" s="3">
+        <v>30951.743137548383</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>3580</v>
       </c>
@@ -21362,8 +21947,17 @@
       <c r="Q64">
         <v>0.37859388972001823</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S64">
+        <v>21.3</v>
+      </c>
+      <c r="T64" s="2">
+        <v>0.18206907727969637</v>
+      </c>
+      <c r="U64" s="3">
+        <v>30951.743137548383</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>4145</v>
       </c>
@@ -21415,8 +22009,17 @@
       <c r="Q65">
         <v>0.43588989435406744</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S65">
+        <v>22.1</v>
+      </c>
+      <c r="T65" s="2">
+        <v>0.13244967481990888</v>
+      </c>
+      <c r="U65" s="3">
+        <v>22516.444719384512</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>4801</v>
       </c>
@@ -21468,8 +22071,17 @@
       <c r="Q66">
         <v>0.46188021535170065</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S66">
+        <v>22.2</v>
+      </c>
+      <c r="T66" s="2">
+        <v>0.13244967481990888</v>
+      </c>
+      <c r="U66" s="3">
+        <v>22516.444719384512</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>5560</v>
       </c>
@@ -21521,8 +22133,17 @@
       <c r="Q67">
         <v>0.46188021535170065</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S67">
+        <v>22.3</v>
+      </c>
+      <c r="T67" s="2">
+        <v>0.13244967481990888</v>
+      </c>
+      <c r="U67" s="3">
+        <v>22516.444719384512</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>6439</v>
       </c>
@@ -21574,8 +22195,17 @@
       <c r="Q68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S68">
+        <v>23.1</v>
+      </c>
+      <c r="T68" s="2">
+        <v>9.6274835887881757E-2</v>
+      </c>
+      <c r="U68" s="3">
+        <v>16366.722100939898</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>7456</v>
       </c>
@@ -21627,8 +22257,17 @@
       <c r="Q69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S69">
+        <v>23.2</v>
+      </c>
+      <c r="T69" s="2">
+        <v>9.6274835887881757E-2</v>
+      </c>
+      <c r="U69" s="3">
+        <v>16366.722100939898</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>8635</v>
       </c>
@@ -21680,8 +22319,17 @@
       <c r="Q70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S70">
+        <v>23.3</v>
+      </c>
+      <c r="T70" s="2">
+        <v>9.6274835887881757E-2</v>
+      </c>
+      <c r="U70" s="3">
+        <v>16366.722100939898</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>10000</v>
       </c>
@@ -21733,6 +22381,23 @@
       <c r="Q71">
         <v>0</v>
       </c>
+      <c r="S71">
+        <v>24.1</v>
+      </c>
+      <c r="T71" s="2">
+        <v>0</v>
+      </c>
+      <c r="U71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T72" s="2"/>
+      <c r="U72" s="3"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T73" s="2"/>
+      <c r="U73" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Double checked clump_sandbox, hcmv_env.yaml file
</commit_message>
<xml_diff>
--- a/data/Experimental_data_Ed_Josh.xlsx
+++ b/data/Experimental_data_Ed_Josh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuamiller/Python Files/HCMV_Dose_Infection/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EB98F5-B1B4-EB4E-AA97-6FABBC81D46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160EACEF-C37D-7B4E-B189-FB392833AD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021_10_05 TB_GFP_epithelial" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="210">
   <si>
     <t>Cells</t>
   </si>
@@ -491,9 +491,6 @@
   </si>
   <si>
     <t>stock/well</t>
-  </si>
-  <si>
-    <t>Genomes/well.1</t>
   </si>
   <si>
     <t>g_GFP=0.10406061188380772</t>
@@ -3710,7 +3707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE92A1AC-35E5-614F-A674-F1A8575ADCFB}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3780,10 +3777,10 @@
         <v>135</v>
       </c>
       <c r="J2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" t="s">
         <v>171</v>
-      </c>
-      <c r="K2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -3815,10 +3812,10 @@
         <v>135</v>
       </c>
       <c r="J3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -3850,10 +3847,10 @@
         <v>135</v>
       </c>
       <c r="J4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -3885,7 +3882,7 @@
         <v>135</v>
       </c>
       <c r="J5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -3917,7 +3914,7 @@
         <v>135</v>
       </c>
       <c r="J6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -3949,7 +3946,7 @@
         <v>135</v>
       </c>
       <c r="J7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -3981,7 +3978,7 @@
         <v>135</v>
       </c>
       <c r="J8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -4013,7 +4010,7 @@
         <v>135</v>
       </c>
       <c r="J9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -4045,7 +4042,7 @@
         <v>135</v>
       </c>
       <c r="J10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -4077,7 +4074,7 @@
         <v>135</v>
       </c>
       <c r="J11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -4109,7 +4106,7 @@
         <v>135</v>
       </c>
       <c r="J12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -4141,7 +4138,7 @@
         <v>135</v>
       </c>
       <c r="J13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -4173,7 +4170,7 @@
         <v>135</v>
       </c>
       <c r="J14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -4205,7 +4202,7 @@
         <v>135</v>
       </c>
       <c r="J15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -4237,7 +4234,7 @@
         <v>135</v>
       </c>
       <c r="J16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -4269,7 +4266,7 @@
         <v>135</v>
       </c>
       <c r="J17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -4301,7 +4298,7 @@
         <v>135</v>
       </c>
       <c r="J18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -4333,7 +4330,7 @@
         <v>135</v>
       </c>
       <c r="J19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -4365,7 +4362,7 @@
         <v>135</v>
       </c>
       <c r="J20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -4397,7 +4394,7 @@
         <v>135</v>
       </c>
       <c r="J21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -4429,7 +4426,7 @@
         <v>135</v>
       </c>
       <c r="J22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -4461,7 +4458,7 @@
         <v>135</v>
       </c>
       <c r="J23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -4493,7 +4490,7 @@
         <v>135</v>
       </c>
       <c r="J24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -4525,7 +4522,7 @@
         <v>135</v>
       </c>
       <c r="J25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -4557,7 +4554,7 @@
         <v>135</v>
       </c>
       <c r="J26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -4589,7 +4586,7 @@
         <v>135</v>
       </c>
       <c r="J27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -4621,7 +4618,7 @@
         <v>135</v>
       </c>
       <c r="J28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -4653,7 +4650,7 @@
         <v>135</v>
       </c>
       <c r="J29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -4685,7 +4682,7 @@
         <v>135</v>
       </c>
       <c r="J30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -4717,7 +4714,7 @@
         <v>135</v>
       </c>
       <c r="J31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -4749,7 +4746,7 @@
         <v>135</v>
       </c>
       <c r="J32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -4781,7 +4778,7 @@
         <v>135</v>
       </c>
       <c r="J33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -4813,7 +4810,7 @@
         <v>135</v>
       </c>
       <c r="J34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -4845,7 +4842,7 @@
         <v>135</v>
       </c>
       <c r="J35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -4877,7 +4874,7 @@
         <v>135</v>
       </c>
       <c r="J36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -4909,7 +4906,7 @@
         <v>135</v>
       </c>
       <c r="J37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -4941,7 +4938,7 @@
         <v>135</v>
       </c>
       <c r="J38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -4973,7 +4970,7 @@
         <v>135</v>
       </c>
       <c r="J39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -5005,7 +5002,7 @@
         <v>135</v>
       </c>
       <c r="J40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -5037,7 +5034,7 @@
         <v>135</v>
       </c>
       <c r="J41" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -5069,7 +5066,7 @@
         <v>135</v>
       </c>
       <c r="J42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -5101,7 +5098,7 @@
         <v>135</v>
       </c>
       <c r="J43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -5133,7 +5130,7 @@
         <v>135</v>
       </c>
       <c r="J44" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -5165,7 +5162,7 @@
         <v>135</v>
       </c>
       <c r="J45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -5197,7 +5194,7 @@
         <v>135</v>
       </c>
       <c r="J46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -5229,7 +5226,7 @@
         <v>135</v>
       </c>
       <c r="J47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -5261,7 +5258,7 @@
         <v>135</v>
       </c>
       <c r="J48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -5293,7 +5290,7 @@
         <v>135</v>
       </c>
       <c r="J49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -5325,7 +5322,7 @@
         <v>135</v>
       </c>
       <c r="J50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -5357,7 +5354,7 @@
         <v>135</v>
       </c>
       <c r="J51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -5389,7 +5386,7 @@
         <v>135</v>
       </c>
       <c r="J52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -5421,7 +5418,7 @@
         <v>135</v>
       </c>
       <c r="J53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -5453,7 +5450,7 @@
         <v>135</v>
       </c>
       <c r="J54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -5485,7 +5482,7 @@
         <v>135</v>
       </c>
       <c r="J55" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -5517,7 +5514,7 @@
         <v>135</v>
       </c>
       <c r="J56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -5549,7 +5546,7 @@
         <v>135</v>
       </c>
       <c r="J57" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -5581,7 +5578,7 @@
         <v>135</v>
       </c>
       <c r="J58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -5613,7 +5610,7 @@
         <v>135</v>
       </c>
       <c r="J59" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -5645,7 +5642,7 @@
         <v>135</v>
       </c>
       <c r="J60" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -5677,7 +5674,7 @@
         <v>135</v>
       </c>
       <c r="J61" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -5709,7 +5706,7 @@
         <v>135</v>
       </c>
       <c r="J62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -5741,7 +5738,7 @@
         <v>135</v>
       </c>
       <c r="J63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -5773,7 +5770,7 @@
         <v>135</v>
       </c>
       <c r="J64" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -5805,7 +5802,7 @@
         <v>135</v>
       </c>
       <c r="J65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -5837,7 +5834,7 @@
         <v>135</v>
       </c>
       <c r="J66" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -5869,7 +5866,7 @@
         <v>135</v>
       </c>
       <c r="J67" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -5901,7 +5898,7 @@
         <v>135</v>
       </c>
       <c r="J68" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
@@ -5933,7 +5930,7 @@
         <v>135</v>
       </c>
       <c r="J69" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
@@ -5965,7 +5962,7 @@
         <v>135</v>
       </c>
       <c r="J70" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -5997,7 +5994,7 @@
         <v>135</v>
       </c>
       <c r="J71" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -6029,7 +6026,7 @@
         <v>135</v>
       </c>
       <c r="J72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -6061,7 +6058,7 @@
         <v>135</v>
       </c>
       <c r="J73" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -6099,55 +6096,55 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>181</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>182</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>183</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>184</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>185</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>186</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>187</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>188</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>189</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>190</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>191</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>192</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>193</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>194</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>195</v>
       </c>
       <c r="S1" t="s">
         <v>126</v>
@@ -10535,76 +10532,76 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="N1" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="R1" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="Q1" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="T1" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="U1" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="T1" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="W1" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="V1" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>209</v>
-      </c>
       <c r="X1" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Z1" t="s">
         <v>126</v>
@@ -21220,7 +21217,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -23813,13 +23812,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -23839,19 +23845,16 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>149</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -23874,19 +23877,16 @@
         <v>9100000</v>
       </c>
       <c r="H2">
-        <v>9100000</v>
+        <v>70</v>
       </c>
       <c r="I2">
-        <v>70</v>
-      </c>
-      <c r="J2">
         <v>0.48886923076923078</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -23909,19 +23909,16 @@
         <v>8400000</v>
       </c>
       <c r="H3">
-        <v>8400000</v>
+        <v>64.615384615384613</v>
       </c>
       <c r="I3">
-        <v>64.615384615384613</v>
-      </c>
-      <c r="J3">
         <v>0.45836153846153849</v>
       </c>
-      <c r="K3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -23934,20 +23931,20 @@
       <c r="D4">
         <v>71333.450869769629</v>
       </c>
+      <c r="G4">
+        <v>8400000</v>
+      </c>
       <c r="H4">
-        <v>8400000</v>
+        <v>64.615384615384613</v>
       </c>
       <c r="I4">
-        <v>64.615384615384613</v>
-      </c>
-      <c r="J4">
         <v>0.5487153846153846</v>
       </c>
-      <c r="K4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -23960,20 +23957,20 @@
       <c r="D5">
         <v>68962.585034013609</v>
       </c>
+      <c r="G5">
+        <v>8400000</v>
+      </c>
       <c r="H5">
-        <v>8400000</v>
+        <v>64.615384615384613</v>
       </c>
       <c r="I5">
-        <v>64.615384615384613</v>
-      </c>
-      <c r="J5">
         <v>0.53048461538461533</v>
       </c>
-      <c r="K5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -23996,19 +23993,16 @@
         <v>7700000</v>
       </c>
       <c r="H6">
-        <v>7700000</v>
+        <v>59.230769230769234</v>
       </c>
       <c r="I6">
-        <v>59.230769230769234</v>
-      </c>
-      <c r="J6">
         <v>0.50013846153846153</v>
       </c>
-      <c r="K6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -24021,20 +24015,20 @@
       <c r="D7">
         <v>60917.338709677417</v>
       </c>
+      <c r="G7">
+        <v>7700000</v>
+      </c>
       <c r="H7">
-        <v>7700000</v>
+        <v>59.230769230769234</v>
       </c>
       <c r="I7">
-        <v>59.230769230769234</v>
-      </c>
-      <c r="J7">
         <v>0.4685923076923077</v>
       </c>
-      <c r="K7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -24047,20 +24041,20 @@
       <c r="D8">
         <v>64598.060920680968</v>
       </c>
+      <c r="G8">
+        <v>7700000</v>
+      </c>
       <c r="H8">
-        <v>7700000</v>
+        <v>59.230769230769234</v>
       </c>
       <c r="I8">
-        <v>59.230769230769234</v>
-      </c>
-      <c r="J8">
         <v>0.49690769230769227</v>
       </c>
-      <c r="K8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -24083,19 +24077,16 @@
         <v>7000000</v>
       </c>
       <c r="H9">
-        <v>7000000</v>
+        <v>53.846153846153847</v>
       </c>
       <c r="I9">
-        <v>53.846153846153847</v>
-      </c>
-      <c r="J9">
         <v>0.46333846153846148</v>
       </c>
-      <c r="K9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -24108,20 +24099,20 @@
       <c r="D10">
         <v>64555.103418530947</v>
       </c>
+      <c r="G10">
+        <v>7000000</v>
+      </c>
       <c r="H10">
-        <v>7000000</v>
+        <v>53.846153846153847</v>
       </c>
       <c r="I10">
-        <v>53.846153846153847</v>
-      </c>
-      <c r="J10">
         <v>0.49657692307692308</v>
       </c>
-      <c r="K10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -24134,17 +24125,17 @@
       <c r="D11">
         <v>60552.12650527402</v>
       </c>
+      <c r="G11">
+        <v>7000000</v>
+      </c>
       <c r="H11">
-        <v>7000000</v>
+        <v>53.846153846153847</v>
       </c>
       <c r="I11">
-        <v>53.846153846153847</v>
-      </c>
-      <c r="J11">
         <v>0.46578461538461541</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -24167,16 +24158,13 @@
         <v>6300000</v>
       </c>
       <c r="H12">
-        <v>6300000</v>
+        <v>48.46153846153846</v>
       </c>
       <c r="I12">
-        <v>48.46153846153846</v>
-      </c>
-      <c r="J12">
         <v>0.47583076923076922</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -24189,17 +24177,17 @@
       <c r="D13">
         <v>57988.33250851067</v>
       </c>
+      <c r="G13">
+        <v>6300000</v>
+      </c>
       <c r="H13">
-        <v>6300000</v>
+        <v>48.46153846153846</v>
       </c>
       <c r="I13">
-        <v>48.46153846153846</v>
-      </c>
-      <c r="J13">
         <v>0.44606153846153851</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -24212,17 +24200,17 @@
       <c r="D14">
         <v>60248.88093106536</v>
       </c>
+      <c r="G14">
+        <v>6300000</v>
+      </c>
       <c r="H14">
-        <v>6300000</v>
+        <v>48.46153846153846</v>
       </c>
       <c r="I14">
-        <v>48.46153846153846</v>
-      </c>
-      <c r="J14">
         <v>0.46345384615384622</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -24245,16 +24233,13 @@
         <v>5600000</v>
       </c>
       <c r="H15">
-        <v>5600000</v>
+        <v>43.07692307692308</v>
       </c>
       <c r="I15">
-        <v>43.07692307692308</v>
-      </c>
-      <c r="J15">
         <v>0.46279999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -24267,17 +24252,17 @@
       <c r="D16">
         <v>54720.006787714243</v>
       </c>
+      <c r="G16">
+        <v>5600000</v>
+      </c>
       <c r="H16">
-        <v>5600000</v>
+        <v>43.07692307692308</v>
       </c>
       <c r="I16">
-        <v>43.07692307692308</v>
-      </c>
-      <c r="J16">
         <v>0.4209230769230769</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -24290,17 +24275,17 @@
       <c r="D17">
         <v>59607.549795598847</v>
       </c>
+      <c r="G17">
+        <v>5600000</v>
+      </c>
       <c r="H17">
-        <v>5600000</v>
+        <v>43.07692307692308</v>
       </c>
       <c r="I17">
-        <v>43.07692307692308</v>
-      </c>
-      <c r="J17">
         <v>0.45852307692307692</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -24323,16 +24308,13 @@
         <v>4900000.0000000009</v>
       </c>
       <c r="H18">
-        <v>4900000.0000000009</v>
+        <v>37.692307692307701</v>
       </c>
       <c r="I18">
-        <v>37.692307692307701</v>
-      </c>
-      <c r="J18">
         <v>0.41623076923076918</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -24345,17 +24327,17 @@
       <c r="D19">
         <v>58796.376186367561</v>
       </c>
+      <c r="G19">
+        <v>4900000.0000000009</v>
+      </c>
       <c r="H19">
-        <v>4900000.0000000009</v>
+        <v>37.692307692307701</v>
       </c>
       <c r="I19">
-        <v>37.692307692307701</v>
-      </c>
-      <c r="J19">
         <v>0.45227692307692308</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -24368,17 +24350,17 @@
       <c r="D20">
         <v>59739.462454143897</v>
       </c>
+      <c r="G20">
+        <v>4900000.0000000009</v>
+      </c>
       <c r="H20">
-        <v>4900000.0000000009</v>
+        <v>37.692307692307701</v>
       </c>
       <c r="I20">
-        <v>37.692307692307701</v>
-      </c>
-      <c r="J20">
         <v>0.45953076923076919</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -24401,16 +24383,13 @@
         <v>4200000</v>
       </c>
       <c r="H21">
-        <v>4200000</v>
+        <v>32.307692307692307</v>
       </c>
       <c r="I21">
-        <v>32.307692307692307</v>
-      </c>
-      <c r="J21">
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -24423,17 +24402,17 @@
       <c r="D22">
         <v>53936.444885799407</v>
       </c>
+      <c r="G22">
+        <v>4200000</v>
+      </c>
       <c r="H22">
-        <v>4200000</v>
+        <v>32.307692307692307</v>
       </c>
       <c r="I22">
-        <v>32.307692307692307</v>
-      </c>
-      <c r="J22">
         <v>0.41489230769230773</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -24456,16 +24435,13 @@
         <v>3500000</v>
       </c>
       <c r="H23">
-        <v>3500000</v>
+        <v>26.92307692307692</v>
       </c>
       <c r="I23">
-        <v>26.92307692307692</v>
-      </c>
-      <c r="J23">
         <v>0.39165384615384607</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -24478,17 +24454,17 @@
       <c r="D24">
         <v>48529.080878864683</v>
       </c>
+      <c r="G24">
+        <v>3500000</v>
+      </c>
       <c r="H24">
-        <v>3500000</v>
+        <v>26.92307692307692</v>
       </c>
       <c r="I24">
-        <v>26.92307692307692</v>
-      </c>
-      <c r="J24">
         <v>0.37330000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -24501,17 +24477,17 @@
       <c r="D25">
         <v>49860.873964459621</v>
       </c>
+      <c r="G25">
+        <v>3500000</v>
+      </c>
       <c r="H25">
-        <v>3500000</v>
+        <v>26.92307692307692</v>
       </c>
       <c r="I25">
-        <v>26.92307692307692</v>
-      </c>
-      <c r="J25">
         <v>0.38354615384615393</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -24534,16 +24510,13 @@
         <v>2800000</v>
       </c>
       <c r="H26">
-        <v>2800000</v>
+        <v>21.53846153846154</v>
       </c>
       <c r="I26">
-        <v>21.53846153846154</v>
-      </c>
-      <c r="J26">
         <v>0.4142769230769231</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -24556,17 +24529,17 @@
       <c r="D27">
         <v>52393.482387681928</v>
       </c>
+      <c r="G27">
+        <v>2800000</v>
+      </c>
       <c r="H27">
-        <v>2800000</v>
+        <v>21.53846153846154</v>
       </c>
       <c r="I27">
-        <v>21.53846153846154</v>
-      </c>
-      <c r="J27">
         <v>0.40302307692307687</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -24579,17 +24552,17 @@
       <c r="D28">
         <v>48620.222098683407</v>
       </c>
+      <c r="G28">
+        <v>2800000</v>
+      </c>
       <c r="H28">
-        <v>2800000</v>
+        <v>21.53846153846154</v>
       </c>
       <c r="I28">
-        <v>21.53846153846154</v>
-      </c>
-      <c r="J28">
         <v>0.374</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -24612,16 +24585,13 @@
         <v>2100000</v>
       </c>
       <c r="H29">
-        <v>2100000</v>
+        <v>16.15384615384615</v>
       </c>
       <c r="I29">
-        <v>16.15384615384615</v>
-      </c>
-      <c r="J29">
         <v>0.34913076923076919</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -24634,17 +24604,17 @@
       <c r="D30">
         <v>52195.917882995127</v>
       </c>
+      <c r="G30">
+        <v>2100000</v>
+      </c>
       <c r="H30">
-        <v>2100000</v>
+        <v>16.15384615384615</v>
       </c>
       <c r="I30">
-        <v>16.15384615384615</v>
-      </c>
-      <c r="J30">
         <v>0.40150769230769229</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -24657,17 +24627,17 @@
       <c r="D31">
         <v>42163.203753351198</v>
       </c>
+      <c r="G31">
+        <v>2100000</v>
+      </c>
       <c r="H31">
-        <v>2100000</v>
+        <v>16.15384615384615</v>
       </c>
       <c r="I31">
-        <v>16.15384615384615</v>
-      </c>
-      <c r="J31">
         <v>0.32433076923076931</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -24690,16 +24660,13 @@
         <v>1400000</v>
       </c>
       <c r="H32">
-        <v>1400000</v>
+        <v>10.76923076923077</v>
       </c>
       <c r="I32">
-        <v>10.76923076923077</v>
-      </c>
-      <c r="J32">
         <v>0.29420769230769228</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -24712,17 +24679,17 @@
       <c r="D33">
         <v>30738.498682668502</v>
       </c>
+      <c r="G33">
+        <v>1400000</v>
+      </c>
       <c r="H33">
-        <v>1400000</v>
+        <v>10.76923076923077</v>
       </c>
       <c r="I33">
-        <v>10.76923076923077</v>
-      </c>
-      <c r="J33">
         <v>0.23644615384615381</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -24735,17 +24702,17 @@
       <c r="D34">
         <v>36323.569212832837</v>
       </c>
+      <c r="G34">
+        <v>1400000</v>
+      </c>
       <c r="H34">
-        <v>1400000</v>
+        <v>10.76923076923077</v>
       </c>
       <c r="I34">
-        <v>10.76923076923077</v>
-      </c>
-      <c r="J34">
         <v>0.27941538461538462</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -24768,16 +24735,13 @@
         <v>700000</v>
       </c>
       <c r="H35">
-        <v>700000</v>
+        <v>5.384615384615385</v>
       </c>
       <c r="I35">
-        <v>5.384615384615385</v>
-      </c>
-      <c r="J35">
         <v>0.1376</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -24790,17 +24754,17 @@
       <c r="D36">
         <v>20777.671178010231</v>
       </c>
+      <c r="G36">
+        <v>700000</v>
+      </c>
       <c r="H36">
-        <v>700000</v>
+        <v>5.384615384615385</v>
       </c>
       <c r="I36">
-        <v>5.384615384615385</v>
-      </c>
-      <c r="J36">
         <v>0.15983076923076919</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -24813,17 +24777,17 @@
       <c r="D37">
         <v>21943.269108540509</v>
       </c>
+      <c r="G37">
+        <v>700000</v>
+      </c>
       <c r="H37">
-        <v>700000</v>
+        <v>5.384615384615385</v>
       </c>
       <c r="I37">
-        <v>5.384615384615385</v>
-      </c>
-      <c r="J37">
         <v>0.16879230769230771</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -24842,17 +24806,17 @@
       <c r="F38">
         <v>0</v>
       </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
         <v>6.9230769230769237E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -24865,17 +24829,17 @@
       <c r="D39">
         <v>7.5214796100402106</v>
       </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
         <v>6.1538461538461535E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -24888,13 +24852,13 @@
       <c r="D40">
         <v>16.33959544837526</v>
       </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
         <v>1.230769230769231E-4</v>
       </c>
     </row>
@@ -24942,19 +24906,19 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>7</v>
@@ -25007,7 +24971,7 @@
         <v>9.8088162995155666E-3</v>
       </c>
       <c r="O2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -25048,7 +25012,7 @@
         <v>9.3994746685879191E-3</v>
       </c>
       <c r="O3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -25089,7 +25053,7 @@
         <v>9.5687527647784678E-3</v>
       </c>
       <c r="O4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -25136,7 +25100,7 @@
         <v>7.4930344472318054E-3</v>
       </c>
       <c r="O5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -25177,7 +25141,7 @@
         <v>7.5899457861015266E-3</v>
       </c>
       <c r="O6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -25218,7 +25182,7 @@
         <v>7.7924930602515496E-3</v>
       </c>
       <c r="O7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -25265,7 +25229,7 @@
         <v>5.9020803320333701E-3</v>
       </c>
       <c r="O8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -25306,7 +25270,7 @@
         <v>5.0572283902533413E-3</v>
       </c>
       <c r="O9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -25347,7 +25311,7 @@
         <v>4.893160168126535E-3</v>
       </c>
       <c r="O10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -26188,10 +26152,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>148</v>
@@ -26209,7 +26173,7 @@
         <v>127</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>148</v>
@@ -26253,7 +26217,7 @@
         <v>250</v>
       </c>
       <c r="L2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -28462,10 +28426,10 @@
         <v>135</v>
       </c>
       <c r="J2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" t="s">
         <v>171</v>
-      </c>
-      <c r="K2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -28497,10 +28461,10 @@
         <v>135</v>
       </c>
       <c r="J3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -28532,10 +28496,10 @@
         <v>135</v>
       </c>
       <c r="J4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -28567,7 +28531,7 @@
         <v>135</v>
       </c>
       <c r="J5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -28599,7 +28563,7 @@
         <v>135</v>
       </c>
       <c r="J6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -28631,7 +28595,7 @@
         <v>135</v>
       </c>
       <c r="J7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -28663,7 +28627,7 @@
         <v>135</v>
       </c>
       <c r="J8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -28695,7 +28659,7 @@
         <v>135</v>
       </c>
       <c r="J9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -28727,7 +28691,7 @@
         <v>135</v>
       </c>
       <c r="J10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -28759,7 +28723,7 @@
         <v>135</v>
       </c>
       <c r="J11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -28791,7 +28755,7 @@
         <v>135</v>
       </c>
       <c r="J12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -28823,7 +28787,7 @@
         <v>135</v>
       </c>
       <c r="J13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -28855,7 +28819,7 @@
         <v>135</v>
       </c>
       <c r="J14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -28887,7 +28851,7 @@
         <v>135</v>
       </c>
       <c r="J15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -28919,7 +28883,7 @@
         <v>135</v>
       </c>
       <c r="J16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -28951,7 +28915,7 @@
         <v>135</v>
       </c>
       <c r="J17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -28983,7 +28947,7 @@
         <v>135</v>
       </c>
       <c r="J18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -29015,7 +28979,7 @@
         <v>135</v>
       </c>
       <c r="J19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -29047,7 +29011,7 @@
         <v>135</v>
       </c>
       <c r="J20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -29079,7 +29043,7 @@
         <v>135</v>
       </c>
       <c r="J21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -29111,7 +29075,7 @@
         <v>135</v>
       </c>
       <c r="J22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -29143,7 +29107,7 @@
         <v>135</v>
       </c>
       <c r="J23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -29175,7 +29139,7 @@
         <v>135</v>
       </c>
       <c r="J24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -29207,7 +29171,7 @@
         <v>135</v>
       </c>
       <c r="J25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -29239,7 +29203,7 @@
         <v>135</v>
       </c>
       <c r="J26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -29271,7 +29235,7 @@
         <v>135</v>
       </c>
       <c r="J27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -29303,7 +29267,7 @@
         <v>135</v>
       </c>
       <c r="J28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -29335,7 +29299,7 @@
         <v>135</v>
       </c>
       <c r="J29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -29367,7 +29331,7 @@
         <v>135</v>
       </c>
       <c r="J30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -29399,7 +29363,7 @@
         <v>135</v>
       </c>
       <c r="J31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -29431,7 +29395,7 @@
         <v>135</v>
       </c>
       <c r="J32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -29463,7 +29427,7 @@
         <v>135</v>
       </c>
       <c r="J33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -29495,7 +29459,7 @@
         <v>135</v>
       </c>
       <c r="J34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -29527,7 +29491,7 @@
         <v>135</v>
       </c>
       <c r="J35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -29559,7 +29523,7 @@
         <v>135</v>
       </c>
       <c r="J36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -29591,7 +29555,7 @@
         <v>135</v>
       </c>
       <c r="J37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -29623,7 +29587,7 @@
         <v>135</v>
       </c>
       <c r="J38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -29655,7 +29619,7 @@
         <v>135</v>
       </c>
       <c r="J39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -29687,7 +29651,7 @@
         <v>135</v>
       </c>
       <c r="J40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -29719,7 +29683,7 @@
         <v>135</v>
       </c>
       <c r="J41" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -29751,7 +29715,7 @@
         <v>135</v>
       </c>
       <c r="J42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -29783,7 +29747,7 @@
         <v>135</v>
       </c>
       <c r="J43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -29815,7 +29779,7 @@
         <v>135</v>
       </c>
       <c r="J44" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -29847,7 +29811,7 @@
         <v>135</v>
       </c>
       <c r="J45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -29879,7 +29843,7 @@
         <v>135</v>
       </c>
       <c r="J46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -29911,7 +29875,7 @@
         <v>135</v>
       </c>
       <c r="J47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -29943,7 +29907,7 @@
         <v>135</v>
       </c>
       <c r="J48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -29975,7 +29939,7 @@
         <v>135</v>
       </c>
       <c r="J49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -30007,7 +29971,7 @@
         <v>135</v>
       </c>
       <c r="J50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -30039,7 +30003,7 @@
         <v>135</v>
       </c>
       <c r="J51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -30071,7 +30035,7 @@
         <v>135</v>
       </c>
       <c r="J52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -30103,7 +30067,7 @@
         <v>135</v>
       </c>
       <c r="J53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -30135,7 +30099,7 @@
         <v>135</v>
       </c>
       <c r="J54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -30167,7 +30131,7 @@
         <v>135</v>
       </c>
       <c r="J55" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -30199,7 +30163,7 @@
         <v>135</v>
       </c>
       <c r="J56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -30231,7 +30195,7 @@
         <v>135</v>
       </c>
       <c r="J57" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -30263,7 +30227,7 @@
         <v>135</v>
       </c>
       <c r="J58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -30295,7 +30259,7 @@
         <v>135</v>
       </c>
       <c r="J59" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -30327,7 +30291,7 @@
         <v>135</v>
       </c>
       <c r="J60" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -30359,7 +30323,7 @@
         <v>135</v>
       </c>
       <c r="J61" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -30391,7 +30355,7 @@
         <v>135</v>
       </c>
       <c r="J62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -30423,7 +30387,7 @@
         <v>135</v>
       </c>
       <c r="J63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -30455,7 +30419,7 @@
         <v>135</v>
       </c>
       <c r="J64" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -30487,7 +30451,7 @@
         <v>135</v>
       </c>
       <c r="J65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -30519,7 +30483,7 @@
         <v>135</v>
       </c>
       <c r="J66" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -30551,7 +30515,7 @@
         <v>135</v>
       </c>
       <c r="J67" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -30583,7 +30547,7 @@
         <v>135</v>
       </c>
       <c r="J68" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
@@ -30615,7 +30579,7 @@
         <v>135</v>
       </c>
       <c r="J69" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
@@ -30647,7 +30611,7 @@
         <v>135</v>
       </c>
       <c r="J70" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -30679,7 +30643,7 @@
         <v>135</v>
       </c>
       <c r="J71" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -30711,7 +30675,7 @@
         <v>135</v>
       </c>
       <c r="J72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -30743,7 +30707,7 @@
         <v>135</v>
       </c>
       <c r="J73" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -30828,10 +30792,10 @@
         <v>135</v>
       </c>
       <c r="J2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -30863,7 +30827,7 @@
         <v>135</v>
       </c>
       <c r="J3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -30895,7 +30859,7 @@
         <v>135</v>
       </c>
       <c r="J4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -30927,7 +30891,7 @@
         <v>135</v>
       </c>
       <c r="J5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -30959,7 +30923,7 @@
         <v>135</v>
       </c>
       <c r="J6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -30991,7 +30955,7 @@
         <v>135</v>
       </c>
       <c r="J7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -31023,7 +30987,7 @@
         <v>135</v>
       </c>
       <c r="J8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -31055,7 +31019,7 @@
         <v>135</v>
       </c>
       <c r="J9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -31087,7 +31051,7 @@
         <v>135</v>
       </c>
       <c r="J10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -31119,7 +31083,7 @@
         <v>135</v>
       </c>
       <c r="J11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -31151,7 +31115,7 @@
         <v>135</v>
       </c>
       <c r="J12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -31183,7 +31147,7 @@
         <v>135</v>
       </c>
       <c r="J13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -31215,7 +31179,7 @@
         <v>135</v>
       </c>
       <c r="J14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -31247,7 +31211,7 @@
         <v>135</v>
       </c>
       <c r="J15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -31279,7 +31243,7 @@
         <v>135</v>
       </c>
       <c r="J16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -31311,7 +31275,7 @@
         <v>135</v>
       </c>
       <c r="J17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -31343,7 +31307,7 @@
         <v>135</v>
       </c>
       <c r="J18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -31375,7 +31339,7 @@
         <v>135</v>
       </c>
       <c r="J19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -31407,7 +31371,7 @@
         <v>135</v>
       </c>
       <c r="J20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -31439,7 +31403,7 @@
         <v>135</v>
       </c>
       <c r="J21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -31471,7 +31435,7 @@
         <v>135</v>
       </c>
       <c r="J22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -31503,7 +31467,7 @@
         <v>135</v>
       </c>
       <c r="J23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -31535,7 +31499,7 @@
         <v>135</v>
       </c>
       <c r="J24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -31567,7 +31531,7 @@
         <v>135</v>
       </c>
       <c r="J25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>